<commit_message>
Construção de gráficos para o paper
</commit_message>
<xml_diff>
--- a/Exoplanets/55Cnc_e/Conversão lat.xlsx
+++ b/Exoplanets/55Cnc_e/Conversão lat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\Exoplanets\55Cnc_e\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C6E5B4-290F-4B69-A6FD-E1929059FAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3107E8-506F-4E29-96A7-471D994D1076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{F010B853-5C37-4295-ACFC-BAB654A3AB5A}"/>
+    <workbookView xWindow="7770" yWindow="2325" windowWidth="13785" windowHeight="11325" xr2:uid="{F010B853-5C37-4295-ACFC-BAB654A3AB5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -524,7 +524,7 @@
   <dimension ref="B1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,14 +562,14 @@
         <v>83.3</v>
       </c>
       <c r="C2" s="2">
-        <v>0.94299999999999995</v>
+        <v>0.95</v>
       </c>
       <c r="D2" s="3">
         <v>1.5440000000000001E-2</v>
       </c>
       <c r="E2" s="1">
         <f>((1.496 * (10^8)) * D2) / (C2 * 696340)</f>
-        <v>3.5175951485285997</v>
+        <v>3.4916760263815467</v>
       </c>
       <c r="F2">
         <f>PI()/180</f>
@@ -577,7 +577,7 @@
       </c>
       <c r="K2">
         <f>(ASIN(E2*COS(B2*F2))) / PI() * 180</f>
-        <v>24.229990964388683</v>
+        <v>24.040131545735598</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
@@ -602,26 +602,26 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2">
-        <v>0.95</v>
+        <v>0.60199999999999998</v>
       </c>
       <c r="D5" s="3">
-        <v>1.5440000000000001E-2</v>
+        <v>5.5899999999999998E-2</v>
       </c>
       <c r="E5">
         <f>(1.496 * (10^8)*D5) / (C5 * 696340)</f>
-        <v>3.4916760263815467</v>
+        <v>19.949203796175105</v>
       </c>
       <c r="K5">
         <f>180*(ACOS((SIN(B5*PI()/180))/E5)) / PI()</f>
-        <v>74.387874007958203</v>
+        <v>89.01764145289971</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="K10">
-        <v>74.387874007958203</v>
+        <v>89.017641452899696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>